<commit_message>
nouveau champ debug : note interne et Ségur REM #23
</commit_message>
<xml_diff>
--- a/src/main/resources/template-segur-requirement-export-avec-colonnes-prepub.xlsx
+++ b/src/main/resources/template-segur-requirement-export-avec-colonnes-prepub.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <r>
       <rPr>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>points de vérification</t>
+  </si>
+  <si>
+    <t>Note interne</t>
+  </si>
+  <si>
+    <t>Rem Ségur</t>
   </si>
   <si>
     <t>NON</t>
@@ -354,10 +360,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
   </numFmts>
   <fonts count="37">
     <font>
@@ -450,7 +456,81 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,67 +545,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -540,10 +560,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -555,43 +583,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -605,10 +603,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -659,85 +665,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,13 +821,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,73 +839,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -862,15 +868,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -882,6 +879,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -904,18 +919,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -936,15 +940,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -959,151 +954,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1565,12 +1571,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Feuil5"/>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" topLeftCell="AF1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.3" defaultRowHeight="15.75" outlineLevelRow="1"/>
@@ -1607,11 +1613,11 @@
     <col min="30" max="30" width="10.2" style="27" customWidth="1"/>
     <col min="31" max="31" width="30.6" style="26" customWidth="1"/>
     <col min="32" max="35" width="15.2" style="28" customWidth="1"/>
-    <col min="36" max="36" width="40.3" style="28" customWidth="1"/>
-    <col min="37" max="16384" width="9.3" style="28"/>
+    <col min="36" max="38" width="40.3" style="28" customWidth="1"/>
+    <col min="39" max="16384" width="9.3" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="1" ht="56.25" customHeight="1" spans="1:36">
+    <row r="1" s="21" customFormat="1" ht="56.25" customHeight="1" spans="1:38">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -1720,99 +1726,111 @@
       <c r="AJ1" s="40" t="s">
         <v>35</v>
       </c>
+      <c r="AK1" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="40" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" ht="210.75" customHeight="1" spans="1:36">
+    <row r="2" ht="210.75" customHeight="1" spans="1:38">
       <c r="A2" s="30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I2" s="36" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K2" s="38" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M2" s="38" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P2" s="39"/>
       <c r="Q2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="R2" s="39"/>
       <c r="S2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="T2" s="39"/>
       <c r="U2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V2" s="39"/>
       <c r="W2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X2" s="39"/>
       <c r="Y2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Z2" s="39"/>
       <c r="AA2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AB2" s="39"/>
       <c r="AC2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AD2" s="39"/>
       <c r="AE2" s="38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AF2" s="39" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AG2" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH2" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI2" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ2" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="AH2" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI2" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ2" s="41" t="s">
-        <v>50</v>
+      <c r="AK2" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL2" s="41" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1853,93 +1871,93 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="110.25" spans="1:29">
       <c r="A2" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>

</xml_diff>